<commit_message>
test llave de ejecución y manejadores de metodos
</commit_message>
<xml_diff>
--- a/info/metodo-objeto-modulo.xlsx
+++ b/info/metodo-objeto-modulo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josem\Desktop\University\2023C\Desarrollo Web II\bakery-project\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D8AAA0-48D6-4F06-9396-783B92CC80D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D9D8B3-1AF4-4A96-A680-4104D683B609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44970" yWindow="0" windowWidth="12735" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>

</xml_diff>